<commit_message>
edit angles range for ard main
</commit_message>
<xml_diff>
--- a/arm_n_cam_mount_api_8_bytes/calib_angles.xlsx
+++ b/arm_n_cam_mount_api_8_bytes/calib_angles.xlsx
@@ -120,10 +120,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -430,8 +430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="S3" sqref="S3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -444,23 +444,23 @@
       <c r="A1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="1"/>
-      <c r="N1" s="1" t="s">
+      <c r="L1" s="2"/>
+      <c r="N1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="1"/>
-      <c r="P1" s="2" t="s">
+      <c r="O1" s="2"/>
+      <c r="P1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="U1" s="1" t="s">
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="U1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="V1" s="1"/>
+      <c r="V1" s="2"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="C2" t="s">
@@ -493,9 +493,9 @@
       <c r="L2" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2" t="s">
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1" t="s">
         <v>18</v>
       </c>
       <c r="S2" t="s">
@@ -549,13 +549,13 @@
         <f>L3-K3</f>
         <v>284</v>
       </c>
-      <c r="P3" s="2">
+      <c r="P3" s="1">
         <v>15</v>
       </c>
-      <c r="Q3" s="2">
+      <c r="Q3" s="1">
         <v>270</v>
       </c>
-      <c r="R3" s="2">
+      <c r="R3" s="1">
         <v>15</v>
       </c>
       <c r="U3">
@@ -615,13 +615,13 @@
         <f t="shared" ref="O4:O9" si="2">L4-K4</f>
         <v>266</v>
       </c>
-      <c r="P4" s="2">
+      <c r="P4" s="1">
         <v>6</v>
       </c>
-      <c r="Q4" s="2">
+      <c r="Q4" s="1">
         <v>261</v>
       </c>
-      <c r="R4" s="2">
+      <c r="R4" s="1">
         <v>6</v>
       </c>
       <c r="U4">
@@ -681,13 +681,13 @@
         <f t="shared" si="2"/>
         <v>260</v>
       </c>
-      <c r="P5" s="2">
+      <c r="P5" s="1">
         <v>3</v>
       </c>
-      <c r="Q5" s="2">
+      <c r="Q5" s="1">
         <v>258</v>
       </c>
-      <c r="R5" s="2">
+      <c r="R5" s="1">
         <v>3</v>
       </c>
       <c r="U5">
@@ -747,13 +747,13 @@
         <f t="shared" si="2"/>
         <v>264</v>
       </c>
-      <c r="P6" s="2">
+      <c r="P6" s="1">
         <v>5</v>
       </c>
-      <c r="Q6" s="2">
+      <c r="Q6" s="1">
         <v>260</v>
       </c>
-      <c r="R6" s="2">
+      <c r="R6" s="1">
         <v>5</v>
       </c>
       <c r="U6">
@@ -797,9 +797,9 @@
       <c r="O7">
         <v>1</v>
       </c>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
       <c r="U7">
         <v>251</v>
       </c>
@@ -851,13 +851,13 @@
         <f t="shared" si="2"/>
         <v>174</v>
       </c>
-      <c r="P8" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="2">
+      <c r="P8" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="1">
         <v>174</v>
       </c>
-      <c r="R8" s="2">
+      <c r="R8" s="1">
         <v>0</v>
       </c>
       <c r="U8">
@@ -913,13 +913,13 @@
         <f t="shared" si="2"/>
         <v>120</v>
       </c>
-      <c r="P9" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="2">
+      <c r="P9" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="1">
         <v>120</v>
       </c>
-      <c r="R9" s="2">
+      <c r="R9" s="1">
         <v>0</v>
       </c>
       <c r="U9">

</xml_diff>

<commit_message>
edit auto servo imu move
</commit_message>
<xml_diff>
--- a/arm_n_cam_mount_api_8_bytes/calib_angles.xlsx
+++ b/arm_n_cam_mount_api_8_bytes/calib_angles.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>min mcs</t>
   </si>
@@ -80,6 +80,33 @@
   </si>
   <si>
     <t>Дипазоны углов  которые подаем на ардутно! На ней больше ничего не делаем!(среднее( = считается как (мин+макс)/2 - среднее положение привода (должно быть, мин = среднее - минимальное рассттрние от среднего до мин или макс, макс= среднее + аналогично)</t>
+  </si>
+  <si>
+    <t>параллельное звено (сингл серво)</t>
+  </si>
+  <si>
+    <t>mcs/ang (-90...90)</t>
+  </si>
+  <si>
+    <t>checck</t>
+  </si>
+  <si>
+    <t>mid+90</t>
+  </si>
+  <si>
+    <t>mid-90</t>
+  </si>
+  <si>
+    <t>mid+max</t>
+  </si>
+  <si>
+    <t>mid-min</t>
+  </si>
+  <si>
+    <t>"+120"</t>
+  </si>
+  <si>
+    <t>"-120"</t>
   </si>
 </sst>
 </file>
@@ -95,7 +122,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -105,6 +132,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -121,12 +154,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -431,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W19"/>
+  <dimension ref="A1:W24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -967,6 +1001,9 @@
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
       <c r="N14">
         <v>1</v>
       </c>
@@ -981,6 +1018,21 @@
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15">
+        <v>-90</v>
+      </c>
+      <c r="E15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15">
+        <v>90</v>
+      </c>
+      <c r="G15" t="s">
+        <v>13</v>
+      </c>
       <c r="N15">
         <v>2</v>
       </c>
@@ -995,6 +1047,24 @@
       </c>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="C16">
+        <v>2386</v>
+      </c>
+      <c r="D16">
+        <v>2077.5</v>
+      </c>
+      <c r="E16">
+        <v>1454.5</v>
+      </c>
+      <c r="F16">
+        <v>822.5</v>
+      </c>
+      <c r="G16">
+        <v>557.5</v>
+      </c>
+      <c r="I16" t="s">
+        <v>23</v>
+      </c>
       <c r="N16">
         <v>3</v>
       </c>
@@ -1008,7 +1078,25 @@
         <v>255</v>
       </c>
     </row>
-    <row r="17" spans="14:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C17">
+        <v>542</v>
+      </c>
+      <c r="D17">
+        <v>468</v>
+      </c>
+      <c r="E17">
+        <v>326</v>
+      </c>
+      <c r="F17">
+        <v>183</v>
+      </c>
+      <c r="G17">
+        <v>116</v>
+      </c>
+      <c r="I17">
+        <v>6.9720000000000004</v>
+      </c>
       <c r="N17">
         <v>4</v>
       </c>
@@ -1019,7 +1107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="14:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:17" x14ac:dyDescent="0.3">
       <c r="N18">
         <v>5</v>
       </c>
@@ -1033,7 +1121,10 @@
         <v>215</v>
       </c>
     </row>
-    <row r="19" spans="14:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="I19" t="s">
+        <v>24</v>
+      </c>
       <c r="N19">
         <v>6</v>
       </c>
@@ -1045,6 +1136,63 @@
       </c>
       <c r="Q19">
         <v>158</v>
+      </c>
+    </row>
+    <row r="20" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="H20" t="s">
+        <v>27</v>
+      </c>
+      <c r="I20" t="s">
+        <v>25</v>
+      </c>
+      <c r="J20" t="s">
+        <v>26</v>
+      </c>
+      <c r="K20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="H21">
+        <f>(E16-G16)/I17</f>
+        <v>128.65748709122201</v>
+      </c>
+      <c r="I21">
+        <f>(E16-F16)/I17</f>
+        <v>90.64830751577739</v>
+      </c>
+      <c r="J21">
+        <f>(E16-D16)/I17</f>
+        <v>-89.357429718875494</v>
+      </c>
+      <c r="K21">
+        <f>(E16-C16)/I17</f>
+        <v>-133.60585197934594</v>
+      </c>
+    </row>
+    <row r="23" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="H23">
+        <v>120</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="H24">
+        <f>120*I17</f>
+        <v>836.6400000000001</v>
+      </c>
+      <c r="J24" s="3">
+        <f>E16-H24</f>
+        <v>617.8599999999999</v>
+      </c>
+      <c r="K24" s="3">
+        <f>E16+H24</f>
+        <v>2291.1400000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>